<commit_message>
fix: updated security label on team-velocity excel
</commit_message>
<xml_diff>
--- a/static/media/scrum-velocity/team-velocity.xlsx
+++ b/static/media/scrum-velocity/team-velocity.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gvieiraschwade/git_clones/personal/personal-website/static/media/scrum-velocity/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2903FA34-C829-D941-94BD-03D22C4FF67D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66022DDC-5878-BA44-95A2-9927E8380D1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,12 +31,14 @@
     <definedName name="WorkedZoom">OFFSET(Data!$C$2, ROWS(SprintTable[])-1, 0, IF(Overview!$B$10="Yes",-Overview!$C$11,-ROWS(SprintTable[])), 1)</definedName>
     <definedName name="YesNo">Base!$A$1:$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -337,19 +339,9 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="10">
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -512,6 +504,16 @@
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -528,7 +530,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -603,7 +605,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -959,7 +961,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236581752"/>
@@ -1032,7 +1034,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="236546960"/>
@@ -1074,7 +1076,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1104,7 +1106,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1118,7 +1120,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1180,7 +1182,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1903,7 +1905,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="238359392"/>
@@ -1976,7 +1978,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="238350816"/>
@@ -2018,7 +2020,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2048,7 +2050,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2062,7 +2064,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2124,7 +2126,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2512,7 +2514,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="164766816"/>
@@ -2585,7 +2587,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="164766424"/>
@@ -2627,7 +2629,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2657,7 +2659,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4437,21 +4439,21 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Commited"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Incomplete"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completed"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Hidden velocity" dataDxfId="9" dataCellStyle="Percent">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Hidden velocity" dataDxfId="8">
       <calculatedColumnFormula>IF(ISBLANK(SprintTable[[#This Row],[Completed]]),SprintTable[[#This Row],[Planned Velocity]], SprintTable[[#This Row],[Completed]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Planned Velocity" dataDxfId="8" dataCellStyle="Percent"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Planned deviation" dataDxfId="7" dataCellStyle="Percent"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Optimistic velocity" dataDxfId="6" dataCellStyle="Percent">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Planned Velocity" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Planned deviation" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Optimistic velocity" dataDxfId="5">
       <calculatedColumnFormula>SprintTable[[#This Row],[Planned Velocity]]+SprintTable[[#This Row],[Planned deviation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Pessimistic velocity" dataDxfId="5" dataCellStyle="Percent">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Pessimistic velocity" dataDxfId="4">
       <calculatedColumnFormula>SprintTable[[#This Row],[Planned Velocity]]-SprintTable[[#This Row],[Planned deviation]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Burn-up" dataDxfId="4" dataCellStyle="Percent"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Optimistic burn-up" dataDxfId="3" dataCellStyle="Percent"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Pessimistic burn-up" dataDxfId="2" dataCellStyle="Percent"/>
-    <tableColumn id="14" xr3:uid="{B1A2F750-7901-1C4C-9770-C36BED7F40C4}" name="Total points of the sprint" dataDxfId="1" dataCellStyle="Percent">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Burn-up" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Optimistic burn-up" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Pessimistic burn-up" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{B1A2F750-7901-1C4C-9770-C36BED7F40C4}" name="Total points of the sprint" dataDxfId="0">
       <calculatedColumnFormula>SprintTable[[#This Row],[Completed]]+SprintTable[[#This Row],[Incomplete]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4889,7 +4891,7 @@
     <mergeCell ref="A9:D9"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:D11">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>OR($B$10="No")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5444,22 +5446,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="2451ae47-9fde-4453-a31b-5fd0b3957dc4">
-      <UserInfo>
-        <DisplayName>Pierre D'OVIDIO</DisplayName>
-        <AccountId>26</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Henry-Charles VEYSSIERE (contractor)</DisplayName>
-        <AccountId>59</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5646,20 +5638,28 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="2451ae47-9fde-4453-a31b-5fd0b3957dc4">
+      <UserInfo>
+        <DisplayName>Pierre D'OVIDIO</DisplayName>
+        <AccountId>26</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Henry-Charles VEYSSIERE (contractor)</DisplayName>
+        <AccountId>59</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD0D6B9-09E6-4C44-ADF0-CE52FA91CC85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4ED87F2-F3CA-4DEA-AC4E-3E481F69CB0F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2451ae47-9fde-4453-a31b-5fd0b3957dc4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5684,9 +5684,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B4ED87F2-F3CA-4DEA-AC4E-3E481F69CB0F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD0D6B9-09E6-4C44-ADF0-CE52FA91CC85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2451ae47-9fde-4453-a31b-5fd0b3957dc4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>